<commit_message>
updated model with new energy balances and integrated timeloop properly
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\flexigrid\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5832D19C-ACF8-449F-AB0E-754D76AC506B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="9"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -26,10 +27,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">boiler!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -392,7 +399,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -458,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -482,6 +489,7 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -762,7 +770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1111,11 +1119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,16 +1181,16 @@
       <c r="D2" s="4">
         <v>15</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="21">
         <v>0</v>
       </c>
       <c r="F2" s="4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="21">
         <v>0</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="21">
         <v>0</v>
       </c>
       <c r="I2" s="4"/>
@@ -1201,16 +1209,16 @@
       <c r="D3" s="4">
         <v>15</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="21">
         <v>2.4</v>
       </c>
       <c r="F3" s="4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="21">
         <v>2.4</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="21">
         <v>2.4</v>
       </c>
       <c r="I3" s="4"/>
@@ -1229,16 +1237,16 @@
       <c r="D4" s="4">
         <v>15</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="21">
         <v>4.8</v>
       </c>
       <c r="F4" s="4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="21">
         <v>3.66</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="21">
         <v>3.66</v>
       </c>
       <c r="I4" s="4"/>
@@ -1257,16 +1265,16 @@
       <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="21">
         <v>6.4</v>
       </c>
       <c r="F5" s="4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="21">
         <v>3.66</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="21">
         <v>3.66</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -1289,16 +1297,16 @@
       <c r="D6" s="4">
         <v>15</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="21">
         <v>8</v>
       </c>
       <c r="F6" s="4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="21">
         <v>3.66</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="21">
         <v>3.66</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -1321,16 +1329,16 @@
       <c r="D7" s="4">
         <v>15</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="21">
         <v>11</v>
       </c>
       <c r="F7" s="4">
         <v>0.95799999999999996</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="21">
         <v>3.66</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="21">
         <v>3.66</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -1353,16 +1361,16 @@
       <c r="D8" s="4">
         <v>15</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="21">
         <v>16</v>
       </c>
       <c r="F8" s="4">
         <v>0.95799999999999996</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="21">
         <v>3.66</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="21">
         <v>3.66</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -1385,16 +1393,16 @@
       <c r="D9">
         <v>15</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="21">
         <v>22</v>
       </c>
       <c r="F9" s="1">
         <v>0.95799999999999996</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="21">
         <v>3.66</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="21">
         <v>3.66</v>
       </c>
       <c r="I9" t="s">
@@ -1408,63 +1416,85 @@
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E13" s="4"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E14" s="4"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E15" s="4"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E16" s="4"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E17" s="4"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E18" s="4"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E19" s="4"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.35">
@@ -1483,7 +1513,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1852,7 +1882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2264,7 +2294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2360,7 +2390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2884,7 +2914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3456,11 +3486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3626,7 +3656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3746,7 +3776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add energy optimized heat pump
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="9"/>
+    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -1114,7 +1114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
@@ -2364,7 +2364,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2451,7 +2451,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="8">
         <f>$R$2+$S$2*B2</f>
@@ -2509,7 +2509,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" ref="D3:D9" si="0">$R$2+$S$2*B3</f>
@@ -2561,7 +2561,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
@@ -2613,7 +2613,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
@@ -2665,7 +2665,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
@@ -2717,7 +2717,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
@@ -2769,7 +2769,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
@@ -2821,7 +2821,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
@@ -2887,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2975,7 +2975,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="8">
         <f>$R$2+$S$2*B2</f>
@@ -3033,7 +3033,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" ref="D3:D10" si="0">$R$2+$S$2*B3</f>
@@ -3085,7 +3085,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="0"/>
@@ -3137,7 +3137,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="0"/>
@@ -3189,7 +3189,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="0"/>
@@ -3241,7 +3241,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="0"/>
@@ -3293,7 +3293,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="0"/>
@@ -3345,7 +3345,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="0"/>
@@ -3397,7 +3397,7 @@
         <v>47</v>
       </c>
       <c r="C10" s="6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
realistic costs and binary variable for battery
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="5"/>
+    <workbookView xWindow="15" yWindow="30" windowWidth="14415" windowHeight="13380" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -769,19 +769,19 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.26953125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -816,7 +816,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -853,7 +853,7 @@
         <v>-5.7599999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -881,7 +881,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -909,7 +909,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -937,7 +937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -965,7 +965,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -993,7 +993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1112,26 +1112,26 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,77 +1160,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="10">
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="C2" s="11">
-        <v>0.01</v>
+        <v>11.8</v>
       </c>
       <c r="D2" s="4">
         <v>15</v>
       </c>
       <c r="E2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F2" s="4">
         <v>0.95499999999999996</v>
       </c>
       <c r="G2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="H2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="20"/>
     </row>
-    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>1180</v>
+        <v>2360</v>
       </c>
       <c r="C3" s="11">
-        <v>11.8</v>
+        <v>23.6</v>
       </c>
       <c r="D3" s="4">
         <v>15</v>
       </c>
       <c r="E3" s="4">
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
       <c r="F3" s="4">
         <v>0.95499999999999996</v>
       </c>
       <c r="G3" s="4">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="H3" s="4">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>2360</v>
+        <v>10880</v>
       </c>
       <c r="C4" s="11">
-        <v>23.6</v>
+        <v>108.8</v>
       </c>
       <c r="D4" s="4">
         <v>15</v>
       </c>
       <c r="E4" s="4">
-        <v>4.8</v>
+        <v>6.4</v>
       </c>
       <c r="F4" s="4">
         <v>0.95499999999999996</v>
@@ -1241,24 +1241,28 @@
       <c r="H4" s="4">
         <v>3.66</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="I4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>10880</v>
+        <v>12000</v>
       </c>
       <c r="C5" s="11">
-        <v>108.8</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4">
         <v>15</v>
       </c>
       <c r="E5" s="4">
-        <v>6.4</v>
+        <v>8</v>
       </c>
       <c r="F5" s="4">
         <v>0.95499999999999996</v>
@@ -1270,30 +1274,30 @@
         <v>3.66</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>12000</v>
+        <v>14300</v>
       </c>
       <c r="C6" s="11">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D6" s="4">
         <v>15</v>
       </c>
       <c r="E6" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4">
-        <v>0.95499999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="G6" s="4">
         <v>3.66</v>
@@ -1302,27 +1306,27 @@
         <v>3.66</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>14300</v>
+        <v>17600</v>
       </c>
       <c r="C7" s="11">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="D7" s="4">
         <v>15</v>
       </c>
       <c r="E7" s="4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4">
         <v>0.95799999999999996</v>
@@ -1334,29 +1338,29 @@
         <v>3.66</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
-        <v>17600</v>
-      </c>
-      <c r="C8" s="11">
-        <v>176</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8" s="2">
+        <v>22000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>220</v>
+      </c>
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="E8" s="4">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.95799999999999996</v>
       </c>
       <c r="G8" s="4">
@@ -1365,116 +1369,84 @@
       <c r="H8" s="4">
         <v>3.66</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>22000</v>
-      </c>
-      <c r="C9" s="2">
-        <v>220</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.66</v>
-      </c>
-      <c r="H9" s="4">
-        <v>3.66</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="I8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1490,19 +1462,19 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -1537,7 +1509,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1574,7 +1546,7 @@
         <v>-0.3639</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1602,7 +1574,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1630,7 +1602,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1658,7 +1630,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1686,7 +1658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1714,7 +1686,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1742,7 +1714,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1770,7 +1742,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1798,7 +1770,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1826,7 +1798,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
@@ -1836,7 +1808,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
@@ -1859,20 +1831,20 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -1907,7 +1879,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1944,7 +1916,7 @@
         <v>500.9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1976,7 +1948,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2007,7 +1979,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2038,7 +2010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2070,7 +2042,7 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2101,7 +2073,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2132,7 +2104,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2163,7 +2135,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2194,68 +2166,68 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D26" s="2"/>
     </row>
   </sheetData>
@@ -2271,19 +2243,19 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -2306,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2330,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2367,27 +2339,27 @@
       <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.26953125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -2443,7 +2415,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2501,7 +2473,7 @@
         <v>881.48</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -2553,7 +2525,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -2605,7 +2577,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2657,7 +2629,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -2709,7 +2681,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -2761,7 +2733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -2813,7 +2785,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -2865,7 +2837,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2875,7 +2847,7 @@
       <c r="G10" s="6"/>
       <c r="P10" s="7"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
     </row>
   </sheetData>
@@ -2887,31 +2859,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.26953125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -2967,7 +2939,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -3025,7 +2997,7 @@
         <v>614.80999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3077,7 +3049,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -3129,7 +3101,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -3181,7 +3153,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3233,7 +3205,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -3285,7 +3257,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -3337,7 +3309,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -3389,7 +3361,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -3441,13 +3413,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F11" s="17"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H15" s="17"/>
     </row>
   </sheetData>
@@ -3463,21 +3435,21 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3509,7 +3481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3542,7 +3514,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -3575,47 +3547,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="F13" s="1"/>
@@ -3633,21 +3605,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3679,7 +3651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3712,32 +3684,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I10" s="12"/>
     </row>
   </sheetData>
@@ -3753,21 +3725,21 @@
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3799,7 +3771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3834,7 +3806,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3869,7 +3841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3904,7 +3876,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3939,7 +3911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -3974,7 +3946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -4009,7 +3981,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -4044,7 +4016,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -4079,7 +4051,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -4114,7 +4086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
integrated grid optimized hp
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E580FFB-8936-44C3-BA46-7BA92E68D400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEDD2A6-DA6B-449C-A18C-0FA6EAFACAAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -1102,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G17" sqref="F1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1151,325 +1151,298 @@
       </c>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <f xml:space="preserve"> 4500 * 1.2</f>
+        <v>5400</v>
       </c>
       <c r="C2" s="5">
-        <f xml:space="preserve"> 0.01 * B2</f>
-        <v>0</v>
+        <f t="shared" ref="C2:C10" si="0" xml:space="preserve"> 0.01 * B2</f>
+        <v>54</v>
       </c>
       <c r="D2" s="5">
         <v>20</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="G2" s="5">
-        <v>0</v>
+        <v>6.4</v>
       </c>
       <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" s="5"/>
+        <v>6.4</v>
+      </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
-        <f xml:space="preserve"> 4500 * 1.2</f>
-        <v>5400</v>
+        <f xml:space="preserve"> 5200 * 1.2</f>
+        <v>6240</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C11" si="0" xml:space="preserve"> 0.01 * B3</f>
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>62.4</v>
       </c>
       <c r="D3" s="5">
         <v>20</v>
       </c>
       <c r="E3" s="5">
-        <v>6.4</v>
+        <v>7.68</v>
       </c>
       <c r="F3" s="5">
         <v>0.95</v>
       </c>
       <c r="G3" s="5">
-        <v>6.4</v>
+        <v>7.68</v>
       </c>
       <c r="H3" s="5">
-        <v>6.4</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
-        <f xml:space="preserve"> 5200 * 1.2</f>
-        <v>6240</v>
+        <f xml:space="preserve"> 6000 * 1.2</f>
+        <v>7200</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="0"/>
-        <v>62.4</v>
+        <v>72</v>
       </c>
       <c r="D4" s="5">
         <v>20</v>
       </c>
       <c r="E4" s="5">
-        <v>7.68</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="F4" s="5">
         <v>0.95</v>
       </c>
       <c r="G4" s="5">
-        <v>7.68</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="H4" s="5">
-        <v>7.68</v>
-      </c>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5">
-        <f xml:space="preserve"> 6000 * 1.2</f>
-        <v>7200</v>
+        <f xml:space="preserve"> 6600 * 1.2</f>
+        <v>7920</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>79.2</v>
       </c>
       <c r="D5" s="5">
         <v>20</v>
       </c>
       <c r="E5" s="5">
-        <v>8.9600000000000009</v>
+        <v>10.24</v>
       </c>
       <c r="F5" s="5">
         <v>0.95</v>
       </c>
       <c r="G5" s="5">
-        <v>8.9600000000000009</v>
+        <v>10.24</v>
       </c>
       <c r="H5" s="5">
-        <v>8.9600000000000009</v>
+        <v>10.24</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
-        <f xml:space="preserve"> 6600 * 1.2</f>
-        <v>7920</v>
+        <f xml:space="preserve"> 7400 * 1.2</f>
+        <v>8880</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>79.2</v>
+        <v>88.8</v>
       </c>
       <c r="D6" s="5">
         <v>20</v>
       </c>
       <c r="E6" s="5">
-        <v>10.24</v>
+        <v>11.52</v>
       </c>
       <c r="F6" s="5">
         <v>0.95</v>
       </c>
       <c r="G6" s="5">
-        <v>10.24</v>
+        <v>11.52</v>
       </c>
       <c r="H6" s="5">
-        <v>10.24</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>111</v>
-      </c>
+        <v>11.52</v>
+      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
-        <f xml:space="preserve"> 7400 * 1.2</f>
-        <v>8880</v>
+        <f>B6*2</f>
+        <v>17760</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>88.8</v>
+        <v>177.6</v>
       </c>
       <c r="D7" s="5">
         <v>20</v>
       </c>
       <c r="E7" s="5">
-        <v>11.52</v>
+        <f>11.52 * 2</f>
+        <v>23.04</v>
       </c>
       <c r="F7" s="5">
         <v>0.95</v>
       </c>
       <c r="G7" s="5">
-        <v>11.52</v>
+        <f>G6*2</f>
+        <v>23.04</v>
       </c>
       <c r="H7" s="5">
-        <v>11.52</v>
-      </c>
-      <c r="I7" s="5"/>
+        <f>H6*2</f>
+        <v>23.04</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
-        <f>B7*2</f>
-        <v>17760</v>
+        <f>B6*3</f>
+        <v>26640</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>177.6</v>
+        <v>266.39999999999998</v>
       </c>
       <c r="D8" s="5">
         <v>20</v>
       </c>
       <c r="E8" s="5">
-        <f>11.52 * 2</f>
-        <v>23.04</v>
+        <f>11.52*3</f>
+        <v>34.56</v>
       </c>
       <c r="F8" s="5">
         <v>0.95</v>
       </c>
       <c r="G8" s="5">
-        <f>G7*2</f>
-        <v>23.04</v>
+        <f>G6*3</f>
+        <v>34.56</v>
       </c>
       <c r="H8" s="5">
-        <f>H7*2</f>
-        <v>23.04</v>
-      </c>
-      <c r="I8" s="5"/>
+        <f>H6*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
-        <f>B7*3</f>
-        <v>26640</v>
+        <f>B6*4</f>
+        <v>35520</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
-        <v>266.39999999999998</v>
+        <v>355.2</v>
       </c>
       <c r="D9" s="5">
         <v>20</v>
       </c>
       <c r="E9" s="5">
-        <f>11.52*3</f>
-        <v>34.56</v>
+        <f>11.52*4</f>
+        <v>46.08</v>
       </c>
       <c r="F9" s="5">
         <v>0.95</v>
       </c>
       <c r="G9" s="5">
-        <f>G7*3</f>
-        <v>34.56</v>
+        <f>G6*4</f>
+        <v>46.08</v>
       </c>
       <c r="H9" s="5">
-        <f>H7*3</f>
-        <v>34.56</v>
+        <f>H6*4</f>
+        <v>46.08</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
-        <f>B7*4</f>
-        <v>35520</v>
+        <f>B6*5</f>
+        <v>44400</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
-        <v>355.2</v>
+        <v>444</v>
       </c>
       <c r="D10" s="5">
         <v>20</v>
       </c>
       <c r="E10" s="5">
-        <f>11.52*4</f>
-        <v>46.08</v>
+        <f>11.52*5</f>
+        <v>57.599999999999994</v>
       </c>
       <c r="F10" s="5">
         <v>0.95</v>
       </c>
       <c r="G10" s="5">
-        <f>G7*4</f>
-        <v>46.08</v>
+        <f>G6*5</f>
+        <v>57.599999999999994</v>
       </c>
       <c r="H10" s="5">
-        <f>H7*4</f>
-        <v>46.08</v>
+        <f>H6*5</f>
+        <v>57.599999999999994</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5">
-        <f>B7*5</f>
-        <v>44400</v>
-      </c>
-      <c r="C11" s="5">
-        <f t="shared" si="0"/>
-        <v>444</v>
-      </c>
-      <c r="D11" s="5">
-        <v>20</v>
-      </c>
-      <c r="E11" s="5">
-        <f>11.52*5</f>
-        <v>57.599999999999994</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="G11" s="5">
-        <f>G7*5</f>
-        <v>57.599999999999994</v>
-      </c>
-      <c r="H11" s="5">
-        <f>H7*5</f>
-        <v>57.599999999999994</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E12" s="4"/>
-      <c r="J12" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J24" s="2"/>
@@ -1500,14 +1473,11 @@
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J34" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{9D8EB94F-F670-4D91-A7BB-0F8314669F0B}"/>
+    <hyperlink ref="I7" r:id="rId1" xr:uid="{F47F0C45-887D-41FF-98DE-83B4DF900CEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Adition of voltage_comparism.py Merged with Master (added hp opts)
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\flexigrid\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrissi\Git\Flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B10D62-380B-4287-A493-A4099EDB2423}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="30" windowWidth="14420" windowHeight="13380" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -26,10 +27,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">boiler!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -392,7 +399,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -762,7 +769,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1111,11 +1118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1160,30 +1167,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="10">
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="C2" s="11">
-        <v>0.01</v>
+        <v>11.8</v>
       </c>
       <c r="D2" s="4">
         <v>15</v>
       </c>
       <c r="E2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F2" s="4">
         <v>0.95499999999999996</v>
       </c>
       <c r="G2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="H2" s="4">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="20"/>
@@ -1193,44 +1200,44 @@
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>1180</v>
+        <v>2360</v>
       </c>
       <c r="C3" s="11">
-        <v>11.8</v>
+        <v>23.6</v>
       </c>
       <c r="D3" s="4">
         <v>15</v>
       </c>
       <c r="E3" s="4">
-        <v>2.4</v>
+        <v>4.8</v>
       </c>
       <c r="F3" s="4">
         <v>0.95499999999999996</v>
       </c>
       <c r="G3" s="4">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="H3" s="4">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="10">
-        <v>2360</v>
+        <v>10880</v>
       </c>
       <c r="C4" s="11">
-        <v>23.6</v>
+        <v>108.8</v>
       </c>
       <c r="D4" s="4">
         <v>15</v>
       </c>
       <c r="E4" s="4">
-        <v>4.8</v>
+        <v>6.4</v>
       </c>
       <c r="F4" s="4">
         <v>0.95499999999999996</v>
@@ -1241,24 +1248,28 @@
       <c r="H4" s="4">
         <v>3.66</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="10">
-        <v>10880</v>
+        <v>12000</v>
       </c>
       <c r="C5" s="11">
-        <v>108.8</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4">
         <v>15</v>
       </c>
       <c r="E5" s="4">
-        <v>6.4</v>
+        <v>8</v>
       </c>
       <c r="F5" s="4">
         <v>0.95499999999999996</v>
@@ -1270,10 +1281,10 @@
         <v>3.66</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1281,19 +1292,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>12000</v>
+        <v>14300</v>
       </c>
       <c r="C6" s="11">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D6" s="4">
         <v>15</v>
       </c>
       <c r="E6" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F6" s="4">
-        <v>0.95499999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="G6" s="4">
         <v>3.66</v>
@@ -1302,10 +1313,10 @@
         <v>3.66</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1313,16 +1324,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="10">
-        <v>14300</v>
+        <v>17600</v>
       </c>
       <c r="C7" s="11">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="D7" s="4">
         <v>15</v>
       </c>
       <c r="E7" s="4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4">
         <v>0.95799999999999996</v>
@@ -1334,29 +1345,29 @@
         <v>3.66</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
-        <v>17600</v>
-      </c>
-      <c r="C8" s="11">
-        <v>176</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="B8" s="2">
+        <v>22000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>220</v>
+      </c>
+      <c r="D8">
         <v>15</v>
       </c>
-      <c r="E8" s="4">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="E8">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1">
         <v>0.95799999999999996</v>
       </c>
       <c r="G8" s="4">
@@ -1365,41 +1376,12 @@
       <c r="H8" s="4">
         <v>3.66</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>22000</v>
-      </c>
-      <c r="C9" s="2">
-        <v>220</v>
-      </c>
-      <c r="D9">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.66</v>
-      </c>
-      <c r="H9" s="4">
-        <v>3.66</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="I8" t="s">
         <v>51</v>
       </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J11" s="2"/>
@@ -1472,9 +1454,6 @@
     </row>
     <row r="34" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1483,7 +1462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1852,7 +1831,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2264,7 +2243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2360,7 +2339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2884,11 +2863,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3456,7 +3435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3626,7 +3605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3746,7 +3725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
ready for problem solving
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEDD2A6-DA6B-449C-A18C-0FA6EAFACAAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD877592-352A-4D74-AB34-92349D4E1B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -1104,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="F1:G17"/>
     </sheetView>
   </sheetViews>
@@ -2365,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2453,7 +2453,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="7">
         <f>$R$2+$S$2*B2</f>
@@ -2511,7 +2511,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:D9" si="0">$R$2+$S$2*B3</f>
@@ -2563,7 +2563,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" si="0"/>
@@ -2615,7 +2615,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
@@ -2667,7 +2667,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
@@ -2719,7 +2719,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
@@ -2771,7 +2771,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
@@ -2823,7 +2823,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
last update incl. evaluation
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chrissi\Git\Flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A654FF-4268-40D3-94E0-52E72062F9D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBF266A-1F96-4883-82A6-13CDF45D115A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="113">
   <si>
     <t>Number</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Wirkungsgraddiskussion</t>
+  </si>
+  <si>
+    <t>hinzugefügt, nicht nach greenakku</t>
   </si>
 </sst>
 </file>
@@ -1102,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1156,27 +1159,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <f xml:space="preserve"> 4500 * 1.2*0.1</f>
-        <v>540</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C10" si="0" xml:space="preserve"> 0.01 * B2</f>
-        <v>5.4</v>
+        <f t="shared" ref="C2:C12" si="0" xml:space="preserve"> 0.01 * B2</f>
+        <v>10</v>
       </c>
       <c r="D2" s="5">
         <v>20</v>
       </c>
       <c r="E2" s="5">
-        <v>6.4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5">
         <v>0.95</v>
       </c>
       <c r="G2" s="5">
-        <v>6.4</v>
+        <v>2</v>
       </c>
       <c r="H2" s="5">
-        <v>6.4</v>
+        <v>2</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -1184,121 +1189,117 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <f xml:space="preserve"> 5200 * 1.2*0.1</f>
-        <v>624</v>
+        <v>2000</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" si="0"/>
-        <v>6.24</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5">
         <v>20</v>
       </c>
       <c r="E3" s="5">
-        <v>7.68</v>
+        <v>4</v>
       </c>
       <c r="F3" s="5">
         <v>0.95</v>
       </c>
       <c r="G3" s="5">
-        <v>7.68</v>
+        <v>4</v>
       </c>
       <c r="H3" s="5">
-        <v>7.68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <f xml:space="preserve"> 6000 * 1.2*0.1</f>
-        <v>720</v>
+        <f xml:space="preserve"> 4500 * 1.2</f>
+        <v>5400</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5">
         <v>20</v>
       </c>
       <c r="E4" s="5">
-        <v>8.9600000000000009</v>
+        <v>6.4</v>
       </c>
       <c r="F4" s="5">
         <v>0.95</v>
       </c>
       <c r="G4" s="5">
-        <v>8.9600000000000009</v>
+        <v>6.4</v>
       </c>
       <c r="H4" s="5">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <f xml:space="preserve"> 6600 * 1.2*0.1</f>
-        <v>792</v>
+        <f xml:space="preserve"> 5200 * 1.2</f>
+        <v>6240</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="0"/>
-        <v>7.92</v>
+        <v>62.4</v>
       </c>
       <c r="D5" s="5">
         <v>20</v>
       </c>
       <c r="E5" s="5">
-        <v>10.24</v>
+        <v>7.68</v>
       </c>
       <c r="F5" s="5">
         <v>0.95</v>
       </c>
       <c r="G5" s="5">
-        <v>10.24</v>
+        <v>7.68</v>
       </c>
       <c r="H5" s="5">
-        <v>10.24</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="5"/>
+        <v>7.68</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <f xml:space="preserve"> 7400 * 1.2*0.1</f>
-        <v>888</v>
+        <f xml:space="preserve"> 6000 * 1.2</f>
+        <v>7200</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>8.8800000000000008</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5">
         <v>20</v>
       </c>
       <c r="E6" s="5">
-        <v>11.52</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="F6" s="5">
         <v>0.95</v>
       </c>
       <c r="G6" s="5">
-        <v>11.52</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="H6" s="5">
-        <v>11.52</v>
-      </c>
-      <c r="I6" s="5"/>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1306,33 +1307,30 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <f>B6*2</f>
-        <v>1776</v>
+        <f xml:space="preserve"> 6600 * 1.2</f>
+        <v>7920</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>17.760000000000002</v>
+        <v>79.2</v>
       </c>
       <c r="D7" s="5">
         <v>20</v>
       </c>
       <c r="E7" s="5">
-        <f>11.52 * 2</f>
-        <v>23.04</v>
+        <v>10.24</v>
       </c>
       <c r="F7" s="5">
         <v>0.95</v>
       </c>
       <c r="G7" s="5">
-        <f>G6*2</f>
-        <v>23.04</v>
+        <v>10.24</v>
       </c>
       <c r="H7" s="5">
-        <f>H6*2</f>
-        <v>23.04</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>108</v>
+        <v>10.24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1341,34 +1339,29 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <f>B6*3</f>
-        <v>2664</v>
+        <f xml:space="preserve"> 7400 * 1.2</f>
+        <v>8880</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>26.64</v>
+        <v>88.8</v>
       </c>
       <c r="D8" s="5">
         <v>20</v>
       </c>
       <c r="E8" s="5">
-        <f>11.52*3</f>
-        <v>34.56</v>
+        <v>11.52</v>
       </c>
       <c r="F8" s="5">
         <v>0.95</v>
       </c>
       <c r="G8" s="5">
-        <f>G6*3</f>
-        <v>34.56</v>
+        <v>11.52</v>
       </c>
       <c r="H8" s="5">
-        <f>H6*3</f>
-        <v>34.56</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>11.52</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1376,32 +1369,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <f>B6*4</f>
-        <v>3552</v>
+        <f>B8*2</f>
+        <v>17760</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
-        <v>35.520000000000003</v>
+        <v>177.6</v>
       </c>
       <c r="D9" s="5">
         <v>20</v>
       </c>
       <c r="E9" s="5">
-        <f>11.52*4</f>
-        <v>46.08</v>
+        <f>11.52 * 2</f>
+        <v>23.04</v>
       </c>
       <c r="F9" s="5">
         <v>0.95</v>
       </c>
       <c r="G9" s="5">
-        <f>G6*4</f>
-        <v>46.08</v>
+        <f>G8*2</f>
+        <v>23.04</v>
       </c>
       <c r="H9" s="5">
-        <f>H6*4</f>
-        <v>46.08</v>
-      </c>
-      <c r="I9" s="5"/>
+        <f>H8*2</f>
+        <v>23.04</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1409,43 +1404,105 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <f>B6*5</f>
-        <v>4440</v>
+        <f>B8*3</f>
+        <v>26640</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
-        <v>44.4</v>
+        <v>266.39999999999998</v>
       </c>
       <c r="D10" s="5">
         <v>20</v>
       </c>
       <c r="E10" s="5">
+        <f>11.52*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G10" s="5">
+        <f>G8*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="H10" s="5">
+        <f>H8*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <f>B8*4</f>
+        <v>35520</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>355.2</v>
+      </c>
+      <c r="D11" s="5">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <f>11.52*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G11" s="5">
+        <f>G8*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="H11" s="5">
+        <f>H8*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B8*5</f>
+        <v>44400</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>444</v>
+      </c>
+      <c r="D12" s="5">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5">
         <f>11.52*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F12" s="5">
         <v>0.95</v>
       </c>
-      <c r="G10" s="5">
-        <f>G6*5</f>
+      <c r="G12" s="5">
+        <f>G8*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="H10" s="5">
-        <f>H6*5</f>
+      <c r="H12" s="5">
+        <f>H8*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E11" s="4"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J24" s="2"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E13" s="4"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="25" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J25" s="2"/>
@@ -1473,11 +1530,17 @@
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J35" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1" xr:uid="{F47F0C45-887D-41FF-98DE-83B4DF900CEC}"/>
+    <hyperlink ref="I9" r:id="rId1" xr:uid="{F47F0C45-887D-41FF-98DE-83B4DF900CEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
starting with new project
</commit_message>
<xml_diff>
--- a/input/devices.xlsx
+++ b/input/devices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\PycharmProjects\flexigrid\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD877592-352A-4D74-AB34-92349D4E1B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17869A2A-5768-49E5-8AD1-C1B1D1D5F367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boiler" sheetId="4" r:id="rId1"/>
@@ -1102,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="F1:G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1156,27 +1156,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <f xml:space="preserve"> 4500 * 1.2</f>
-        <v>5400</v>
+        <v>1350</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C10" si="0" xml:space="preserve"> 0.01 * B2</f>
-        <v>54</v>
+        <v>13.5</v>
       </c>
       <c r="D2" s="5">
         <v>20</v>
       </c>
       <c r="E2" s="5">
-        <v>6.4</v>
+        <v>1.6</v>
       </c>
       <c r="F2" s="5">
         <v>0.95</v>
       </c>
       <c r="G2" s="5">
-        <v>6.4</v>
+        <v>1.6</v>
       </c>
       <c r="H2" s="5">
-        <v>6.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -1184,121 +1182,113 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
+        <v>2700</v>
+      </c>
+      <c r="C3" s="5">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <f xml:space="preserve"> 4500 * 1.2</f>
+        <v>5400</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:C12" si="0" xml:space="preserve"> 0.01 * B4</f>
+        <v>54</v>
+      </c>
+      <c r="D4" s="5">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
         <f xml:space="preserve"> 5200 * 1.2</f>
         <v>6240</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C5" s="5">
         <f t="shared" si="0"/>
         <v>62.4</v>
       </c>
-      <c r="D3" s="5">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5">
         <v>7.68</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="G3" s="5">
-        <v>7.68</v>
-      </c>
-      <c r="H3" s="5">
-        <v>7.68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <f xml:space="preserve"> 6000 * 1.2</f>
-        <v>7200</v>
-      </c>
-      <c r="C4" s="5">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="D4" s="5">
-        <v>20</v>
-      </c>
-      <c r="E4" s="5">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="G4" s="5">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="H4" s="5">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <f xml:space="preserve"> 6600 * 1.2</f>
-        <v>7920</v>
-      </c>
-      <c r="C5" s="5">
-        <f t="shared" si="0"/>
-        <v>79.2</v>
-      </c>
-      <c r="D5" s="5">
-        <v>20</v>
-      </c>
-      <c r="E5" s="5">
-        <v>10.24</v>
       </c>
       <c r="F5" s="5">
         <v>0.95</v>
       </c>
       <c r="G5" s="5">
-        <v>10.24</v>
+        <v>7.68</v>
       </c>
       <c r="H5" s="5">
-        <v>10.24</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" s="5"/>
+        <v>7.68</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <f xml:space="preserve"> 7400 * 1.2</f>
-        <v>8880</v>
+        <f xml:space="preserve"> 6000 * 1.2</f>
+        <v>7200</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>88.8</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5">
         <v>20</v>
       </c>
       <c r="E6" s="5">
-        <v>11.52</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="F6" s="5">
         <v>0.95</v>
       </c>
       <c r="G6" s="5">
-        <v>11.52</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="H6" s="5">
-        <v>11.52</v>
-      </c>
-      <c r="I6" s="5"/>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1306,33 +1296,30 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <f>B6*2</f>
-        <v>17760</v>
+        <f xml:space="preserve"> 6600 * 1.2</f>
+        <v>7920</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>177.6</v>
+        <v>79.2</v>
       </c>
       <c r="D7" s="5">
         <v>20</v>
       </c>
       <c r="E7" s="5">
-        <f>11.52 * 2</f>
-        <v>23.04</v>
+        <v>10.24</v>
       </c>
       <c r="F7" s="5">
         <v>0.95</v>
       </c>
       <c r="G7" s="5">
-        <f>G6*2</f>
-        <v>23.04</v>
+        <v>10.24</v>
       </c>
       <c r="H7" s="5">
-        <f>H6*2</f>
-        <v>23.04</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>108</v>
+        <v>10.24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="J7" s="5"/>
     </row>
@@ -1341,34 +1328,29 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <f>B6*3</f>
-        <v>26640</v>
+        <f xml:space="preserve"> 7400 * 1.2</f>
+        <v>8880</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
-        <v>266.39999999999998</v>
+        <v>88.8</v>
       </c>
       <c r="D8" s="5">
         <v>20</v>
       </c>
       <c r="E8" s="5">
-        <f>11.52*3</f>
-        <v>34.56</v>
+        <v>11.52</v>
       </c>
       <c r="F8" s="5">
         <v>0.95</v>
       </c>
       <c r="G8" s="5">
-        <f>G6*3</f>
-        <v>34.56</v>
+        <v>11.52</v>
       </c>
       <c r="H8" s="5">
-        <f>H6*3</f>
-        <v>34.56</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>11.52</v>
+      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1376,32 +1358,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <f>B6*4</f>
-        <v>35520</v>
+        <f>B8*2</f>
+        <v>17760</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
-        <v>355.2</v>
+        <v>177.6</v>
       </c>
       <c r="D9" s="5">
         <v>20</v>
       </c>
       <c r="E9" s="5">
-        <f>11.52*4</f>
-        <v>46.08</v>
+        <f>11.52 * 2</f>
+        <v>23.04</v>
       </c>
       <c r="F9" s="5">
         <v>0.95</v>
       </c>
       <c r="G9" s="5">
-        <f>G6*4</f>
-        <v>46.08</v>
+        <f>G8*2</f>
+        <v>23.04</v>
       </c>
       <c r="H9" s="5">
-        <f>H6*4</f>
-        <v>46.08</v>
-      </c>
-      <c r="I9" s="5"/>
+        <f>H8*2</f>
+        <v>23.04</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1409,43 +1393,105 @@
         <v>9</v>
       </c>
       <c r="B10" s="5">
-        <f>B6*5</f>
-        <v>44400</v>
+        <f>B8*3</f>
+        <v>26640</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
+        <v>266.39999999999998</v>
+      </c>
+      <c r="D10" s="5">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5">
+        <f>11.52*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G10" s="5">
+        <f>G8*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="H10" s="5">
+        <f>H8*3</f>
+        <v>34.56</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <f>B8*4</f>
+        <v>35520</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="0"/>
+        <v>355.2</v>
+      </c>
+      <c r="D11" s="5">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <f>11.52*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="G11" s="5">
+        <f>G8*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="H11" s="5">
+        <f>H8*4</f>
+        <v>46.08</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <f>B8*5</f>
+        <v>44400</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
         <v>444</v>
       </c>
-      <c r="D10" s="5">
-        <v>20</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D12" s="5">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5">
         <f>11.52*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F12" s="5">
         <v>0.95</v>
       </c>
-      <c r="G10" s="5">
-        <f>G6*5</f>
+      <c r="G12" s="5">
+        <f>G8*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="H10" s="5">
-        <f>H6*5</f>
+      <c r="H12" s="5">
+        <f>H8*5</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E11" s="4"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="23" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J24" s="2"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E13" s="4"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="25" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J25" s="2"/>
@@ -1473,11 +1519,17 @@
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.35">
+      <c r="J35" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I7" r:id="rId1" xr:uid="{F47F0C45-887D-41FF-98DE-83B4DF900CEC}"/>
+    <hyperlink ref="I9" r:id="rId1" xr:uid="{F47F0C45-887D-41FF-98DE-83B4DF900CEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -2365,7 +2417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>